<commit_message>
Added health state occupancy
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.padgett\_R_\R_PSM_example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ED9F36-D339-4A39-A704-EF883EEB0A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DB0B64-A165-4D19-80DC-C6B24AA76BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-49725" yWindow="1020" windowWidth="23010" windowHeight="12210" xr2:uid="{5C31BBB1-D3A4-45DA-9CBB-5D70D5C11B5C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="240">
   <si>
     <t>SE</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>benefit_discount</t>
+  </si>
+  <si>
+    <t>cohort</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5B7671-BDCF-4EC0-8DF3-19573C2A48D6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,6 +1222,23 @@
         <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
     </row>

</xml_diff>